<commit_message>
added units to formatted data
</commit_message>
<xml_diff>
--- a/exp7/data/readings_formatted.xlsx
+++ b/exp7/data/readings_formatted.xlsx
@@ -13,12 +13,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$58:$F$91</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
   <si>
     <t>l [cm]</t>
   </si>
@@ -56,15 +55,6 @@
     <t>Federtiefe [cm]</t>
   </si>
   <si>
-    <t>T_s</t>
-  </si>
-  <si>
-    <t>phi1</t>
-  </si>
-  <si>
-    <t>phi2</t>
-  </si>
-  <si>
     <t>k</t>
   </si>
   <si>
@@ -92,7 +82,28 @@
     <t>dx1[cm]</t>
   </si>
   <si>
-    <t>dx_2[cm]</t>
+    <t>dx2[cm]</t>
+  </si>
+  <si>
+    <t>Tges [s]</t>
+  </si>
+  <si>
+    <t>T [s]</t>
+  </si>
+  <si>
+    <t>T_s [s]</t>
+  </si>
+  <si>
+    <t>f [Hz]</t>
+  </si>
+  <si>
+    <t>w [rad/s]</t>
+  </si>
+  <si>
+    <t>phi1 [°]</t>
+  </si>
+  <si>
+    <t>phi2 [°]</t>
   </si>
 </sst>
 </file>
@@ -552,7 +563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
       <selection activeCell="A58" sqref="A58:F91"/>
     </sheetView>
   </sheetViews>
@@ -619,7 +630,7 @@
     <row r="9" spans="1:7" ht="12.2" customHeight="1"/>
     <row r="10" spans="1:7" ht="12.6" customHeight="1">
       <c r="B10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -698,7 +709,7 @@
     </row>
     <row r="17" spans="1:6" ht="13.35" customHeight="1">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>20</v>
@@ -707,22 +718,22 @@
     <row r="18" spans="1:6" ht="12.2" customHeight="1"/>
     <row r="19" spans="1:6" ht="13.35" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.2" customHeight="1">
@@ -795,22 +806,22 @@
     <row r="25" spans="1:6" ht="12.2" customHeight="1"/>
     <row r="26" spans="1:6" ht="12.2" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12.2" customHeight="1">
@@ -917,22 +928,22 @@
     <row r="34" spans="1:6" ht="12.2" customHeight="1"/>
     <row r="35" spans="1:6" ht="12.2" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="12.2" customHeight="1">
@@ -1039,22 +1050,22 @@
     <row r="43" spans="1:6" ht="12.2" customHeight="1"/>
     <row r="44" spans="1:6" ht="12.2" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="12.2" customHeight="1">
@@ -1127,22 +1138,22 @@
     <row r="50" spans="1:6" ht="12.2" customHeight="1"/>
     <row r="51" spans="1:6" ht="12.2" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="12.2" customHeight="1">
@@ -1185,22 +1196,22 @@
     <row r="57" spans="1:6" ht="12.2" customHeight="1"/>
     <row r="58" spans="1:6" ht="12.2" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="12.75" customHeight="1">
@@ -1271,22 +1282,22 @@
     </row>
     <row r="65" spans="1:6" ht="12.75" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="12.75" customHeight="1">
@@ -1391,22 +1402,22 @@
     </row>
     <row r="74" spans="1:6" ht="12.75" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="12.75" customHeight="1">
@@ -1511,22 +1522,22 @@
     </row>
     <row r="83" spans="1:6" ht="12.75" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="12.75" customHeight="1">
@@ -1597,22 +1608,22 @@
     </row>
     <row r="90" spans="1:6" ht="12.75" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="12.75" customHeight="1">

</xml_diff>

<commit_message>
Revert "Revert "new diagrams""
This reverts commit 52453592db6e7cf2bc5ba22158ad6a8a0cee8eaa.
</commit_message>
<xml_diff>
--- a/exp7/data/readings_formatted.xlsx
+++ b/exp7/data/readings_formatted.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
   <si>
     <t>l [cm]</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>phi2 [°]</t>
+  </si>
+  <si>
+    <t>(bis mitte gewicht)</t>
   </si>
 </sst>
 </file>
@@ -561,16 +564,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G91"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:F91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
     <col min="5" max="7" width="14.28515625" customWidth="1"/>
@@ -584,7 +587,12 @@
     <col min="18" max="1024" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="12.75" customHeight="1">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="12.75" customHeight="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -598,7 +606,7 @@
         <v>3.14159265358979</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.35" customHeight="1">
+    <row r="4" spans="1:6" ht="13.35" customHeight="1">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -609,7 +617,7 @@
         <v>21.37</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.35" customHeight="1">
+    <row r="5" spans="1:6" ht="13.35" customHeight="1">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -617,7 +625,7 @@
         <v>214.15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.35" customHeight="1">
+    <row r="6" spans="1:6" ht="13.35" customHeight="1">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -625,85 +633,92 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="12.2" customHeight="1"/>
-    <row r="8" spans="1:7" ht="12.2" customHeight="1"/>
-    <row r="9" spans="1:7" ht="12.2" customHeight="1"/>
-    <row r="10" spans="1:7" ht="12.6" customHeight="1">
-      <c r="B10" t="s">
+    <row r="7" spans="1:6" ht="12.2" customHeight="1"/>
+    <row r="8" spans="1:6" ht="12.2" customHeight="1"/>
+    <row r="9" spans="1:6" ht="12.2" customHeight="1"/>
+    <row r="10" spans="1:6" ht="12.6" customHeight="1">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G10" t="s">
+      <c r="F10" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.2" customHeight="1">
-      <c r="C11">
+    <row r="11" spans="1:6" ht="12.2" customHeight="1">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8">
         <v>20</v>
       </c>
-      <c r="D11">
+      <c r="C11" s="8">
         <v>21</v>
       </c>
-      <c r="E11">
+      <c r="D11" s="8">
         <v>1.05</v>
       </c>
-      <c r="F11">
+      <c r="E11" s="8">
         <v>0.952380952380952</v>
       </c>
-      <c r="G11">
+      <c r="F11" s="9">
         <v>5.9839860068377</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="12.2" customHeight="1">
-      <c r="D12">
+    <row r="12" spans="1:6" ht="12.2" customHeight="1">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8">
         <v>20.8</v>
       </c>
-      <c r="E12">
+      <c r="D12" s="8">
         <v>1.04</v>
       </c>
-      <c r="F12">
+      <c r="E12" s="8">
         <v>0.96153846153846101</v>
       </c>
-      <c r="G12">
+      <c r="F12" s="9">
         <v>6.0415243338265201</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.2" customHeight="1">
-      <c r="D13">
+    <row r="13" spans="1:6" ht="12.2" customHeight="1">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8">
         <v>21</v>
       </c>
-      <c r="E13">
+      <c r="D13" s="8">
         <v>1.05</v>
       </c>
-      <c r="F13">
+      <c r="E13" s="8">
         <v>0.952380952380952</v>
       </c>
-      <c r="G13">
+      <c r="F13" s="9">
         <v>5.9839860068377</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="12.2" customHeight="1">
-      <c r="D14">
+    <row r="14" spans="1:6" ht="12.2" customHeight="1">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5">
         <v>21</v>
       </c>
-      <c r="E14">
+      <c r="D14" s="5">
         <v>1.05</v>
       </c>
-      <c r="F14">
+      <c r="E14" s="5">
         <v>0.952380952380952</v>
       </c>
-      <c r="G14">
+      <c r="F14" s="6">
         <v>5.9839860068377</v>
       </c>
     </row>

</xml_diff>